<commit_message>
ajustando tidy armas rio
</commit_message>
<xml_diff>
--- a/inst/tabelas_depara/depara_tipo.xlsx
+++ b/inst/tabelas_depara/depara_tipo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernandopoliano/projetos.R/isdp.armas/inst/tabelas_depara/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wamorim/Documents/institutosoudapaz/isdp.armas/inst/tabelas_depara/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5AFE3A47-BAAE-724E-B441-5E9A89A56D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677664AB-E230-2541-8B77-BD69578D49A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34200" windowHeight="21380" xr2:uid="{67026CC4-D6C3-234F-8EA0-501E1ECEBBD2}"/>
+    <workbookView xWindow="40520" yWindow="7340" windowWidth="19760" windowHeight="13660" xr2:uid="{67026CC4-D6C3-234F-8EA0-501E1ECEBBD2}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="39">
   <si>
     <t>tipo</t>
   </si>
@@ -144,6 +143,15 @@
   </si>
   <si>
     <t>submetralhadora</t>
+  </si>
+  <si>
+    <t>revólver</t>
+  </si>
+  <si>
+    <t>outros</t>
+  </si>
+  <si>
+    <t>garruchão</t>
   </si>
 </sst>
 </file>
@@ -529,14 +537,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3BC569C-3A2A-2D4B-BFBA-4EEB0F78EFA9}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C23"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -781,6 +790,124 @@
         <v>7</v>
       </c>
     </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>